<commit_message>
class imabalance handling results
</commit_message>
<xml_diff>
--- a/experiments/droptc/sentence/DroPTC-all-MiniLM-L6-v2-sentence/freeze/ce-uniform/14298463/prediction.xlsx
+++ b/experiments/droptc/sentence/DroPTC-all-MiniLM-L6-v2-sentence/freeze/ce-uniform/14298463/prediction.xlsx
@@ -490,7 +490,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.991929292678833</v>
+        <v>0.9920104742050171</v>
       </c>
     </row>
     <row r="3">
@@ -518,7 +518,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9900535345077515</v>
+        <v>0.9901875853538513</v>
       </c>
     </row>
     <row r="4">
@@ -546,7 +546,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9908855557441711</v>
+        <v>0.9910318851470947</v>
       </c>
     </row>
     <row r="5">
@@ -574,7 +574,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.923552930355072</v>
+        <v>0.896575927734375</v>
       </c>
     </row>
     <row r="6">
@@ -602,7 +602,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9910865426063538</v>
+        <v>0.9911824464797974</v>
       </c>
     </row>
     <row r="7">
@@ -630,7 +630,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9916369318962097</v>
+        <v>0.9917003512382507</v>
       </c>
     </row>
     <row r="8">
@@ -658,7 +658,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>0.9926276803016663</v>
+        <v>0.9926987290382385</v>
       </c>
     </row>
     <row r="9">
@@ -686,7 +686,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9916501045227051</v>
+        <v>0.9917336702346802</v>
       </c>
     </row>
     <row r="10">
@@ -714,7 +714,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9926276803016663</v>
+        <v>0.9926987290382385</v>
       </c>
     </row>
     <row r="11">
@@ -742,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0.9927496910095215</v>
+        <v>0.9928355813026428</v>
       </c>
     </row>
     <row r="12">
@@ -770,7 +770,7 @@
         <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>0.993091344833374</v>
+        <v>0.9931592345237732</v>
       </c>
     </row>
     <row r="13">
@@ -798,7 +798,7 @@
         <v>1</v>
       </c>
       <c r="F13" t="n">
-        <v>0.968014121055603</v>
+        <v>0.9721521139144897</v>
       </c>
     </row>
     <row r="14">
@@ -826,7 +826,7 @@
         <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>0.9922201037406921</v>
+        <v>0.9923227429389954</v>
       </c>
     </row>
     <row r="15">
@@ -854,7 +854,7 @@
         <v>1</v>
       </c>
       <c r="F15" t="n">
-        <v>0.9916553497314453</v>
+        <v>0.9918570518493652</v>
       </c>
     </row>
     <row r="16">
@@ -882,7 +882,7 @@
         <v>1</v>
       </c>
       <c r="F16" t="n">
-        <v>0.9909260272979736</v>
+        <v>0.9910293817520142</v>
       </c>
     </row>
     <row r="17">
@@ -910,7 +910,7 @@
         <v>1</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9911120533943176</v>
+        <v>0.9912065863609314</v>
       </c>
     </row>
     <row r="18">
@@ -938,7 +938,7 @@
         <v>1</v>
       </c>
       <c r="F18" t="n">
-        <v>0.8035494089126587</v>
+        <v>0.7070009708404541</v>
       </c>
     </row>
     <row r="19">
@@ -966,7 +966,7 @@
         <v>1</v>
       </c>
       <c r="F19" t="n">
-        <v>0.9920235872268677</v>
+        <v>0.9920874238014221</v>
       </c>
     </row>
     <row r="20">
@@ -994,7 +994,7 @@
         <v>1</v>
       </c>
       <c r="F20" t="n">
-        <v>0.993025541305542</v>
+        <v>0.9931128621101379</v>
       </c>
     </row>
     <row r="21">
@@ -1022,7 +1022,7 @@
         <v>1</v>
       </c>
       <c r="F21" t="n">
-        <v>0.9915436506271362</v>
+        <v>0.9916568994522095</v>
       </c>
     </row>
     <row r="22">
@@ -1050,7 +1050,7 @@
         <v>1</v>
       </c>
       <c r="F22" t="n">
-        <v>0.9922882318496704</v>
+        <v>0.992354154586792</v>
       </c>
     </row>
     <row r="23">
@@ -1078,7 +1078,7 @@
         <v>1</v>
       </c>
       <c r="F23" t="n">
-        <v>0.9920090436935425</v>
+        <v>0.9920786023139954</v>
       </c>
     </row>
     <row r="24">
@@ -1106,7 +1106,7 @@
         <v>1</v>
       </c>
       <c r="F24" t="n">
-        <v>0.9923238754272461</v>
+        <v>0.992403507232666</v>
       </c>
     </row>
     <row r="25">
@@ -1134,7 +1134,7 @@
         <v>1</v>
       </c>
       <c r="F25" t="n">
-        <v>0.9353384375572205</v>
+        <v>0.9118024706840515</v>
       </c>
     </row>
     <row r="26">
@@ -1162,7 +1162,7 @@
         <v>1</v>
       </c>
       <c r="F26" t="n">
-        <v>0.6896505951881409</v>
+        <v>0.5855119228363037</v>
       </c>
     </row>
     <row r="27">
@@ -1190,7 +1190,7 @@
         <v>1</v>
       </c>
       <c r="F27" t="n">
-        <v>0.9920002222061157</v>
+        <v>0.9920691251754761</v>
       </c>
     </row>
     <row r="28">
@@ -1218,7 +1218,7 @@
         <v>1</v>
       </c>
       <c r="F28" t="n">
-        <v>0.9900535345077515</v>
+        <v>0.9901875853538513</v>
       </c>
     </row>
     <row r="29">
@@ -1246,7 +1246,7 @@
         <v>1</v>
       </c>
       <c r="F29" t="n">
-        <v>0.9916620254516602</v>
+        <v>0.9917437434196472</v>
       </c>
     </row>
     <row r="30">
@@ -1274,7 +1274,7 @@
         <v>1</v>
       </c>
       <c r="F30" t="n">
-        <v>0.9910945892333984</v>
+        <v>0.9911743402481079</v>
       </c>
     </row>
     <row r="31">
@@ -1302,7 +1302,7 @@
         <v>1</v>
       </c>
       <c r="F31" t="n">
-        <v>0.990071177482605</v>
+        <v>0.9901911020278931</v>
       </c>
     </row>
     <row r="32">
@@ -1330,7 +1330,7 @@
         <v>1</v>
       </c>
       <c r="F32" t="n">
-        <v>0.9917234778404236</v>
+        <v>0.9918311238288879</v>
       </c>
     </row>
     <row r="33">
@@ -1358,7 +1358,7 @@
         <v>1</v>
       </c>
       <c r="F33" t="n">
-        <v>0.971385657787323</v>
+        <v>0.9780473113059998</v>
       </c>
     </row>
     <row r="34">
@@ -1386,7 +1386,7 @@
         <v>1</v>
       </c>
       <c r="F34" t="n">
-        <v>0.9694064259529114</v>
+        <v>0.9730355739593506</v>
       </c>
     </row>
     <row r="35">
@@ -1414,7 +1414,7 @@
         <v>1</v>
       </c>
       <c r="F35" t="n">
-        <v>0.9635248184204102</v>
+        <v>0.9679531455039978</v>
       </c>
     </row>
     <row r="36">
@@ -1442,7 +1442,7 @@
         <v>1</v>
       </c>
       <c r="F36" t="n">
-        <v>0.9916804432868958</v>
+        <v>0.9917593598365784</v>
       </c>
     </row>
     <row r="37">
@@ -1470,7 +1470,7 @@
         <v>1</v>
       </c>
       <c r="F37" t="n">
-        <v>0.9658098220825195</v>
+        <v>0.970139741897583</v>
       </c>
     </row>
     <row r="38">
@@ -1498,7 +1498,7 @@
         <v>1</v>
       </c>
       <c r="F38" t="n">
-        <v>0.9926988482475281</v>
+        <v>0.9927621483802795</v>
       </c>
     </row>
     <row r="39">
@@ -1526,7 +1526,7 @@
         <v>1</v>
       </c>
       <c r="F39" t="n">
-        <v>0.9071575403213501</v>
+        <v>0.9068568348884583</v>
       </c>
     </row>
     <row r="40">
@@ -1554,7 +1554,7 @@
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>0.9714573621749878</v>
+        <v>0.9784333109855652</v>
       </c>
     </row>
     <row r="41">
@@ -1582,7 +1582,7 @@
         <v>1</v>
       </c>
       <c r="F41" t="n">
-        <v>0.9926970601081848</v>
+        <v>0.9927797913551331</v>
       </c>
     </row>
     <row r="42">
@@ -1610,7 +1610,7 @@
         <v>1</v>
       </c>
       <c r="F42" t="n">
-        <v>0.9602239727973938</v>
+        <v>0.9646545648574829</v>
       </c>
     </row>
     <row r="43">
@@ -1638,7 +1638,7 @@
         <v>1</v>
       </c>
       <c r="F43" t="n">
-        <v>0.9684131741523743</v>
+        <v>0.9757384657859802</v>
       </c>
     </row>
     <row r="44">
@@ -1666,7 +1666,7 @@
         <v>1</v>
       </c>
       <c r="F44" t="n">
-        <v>0.9587565660476685</v>
+        <v>0.9635577797889709</v>
       </c>
     </row>
     <row r="45">
@@ -1694,7 +1694,7 @@
         <v>1</v>
       </c>
       <c r="F45" t="n">
-        <v>0.9734935760498047</v>
+        <v>0.9799801111221313</v>
       </c>
     </row>
     <row r="46">
@@ -1722,7 +1722,7 @@
         <v>1</v>
       </c>
       <c r="F46" t="n">
-        <v>0.9690231680870056</v>
+        <v>0.9764753580093384</v>
       </c>
     </row>
     <row r="47">
@@ -1750,7 +1750,7 @@
         <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>0.6729639172554016</v>
+        <v>0.6340534687042236</v>
       </c>
     </row>
     <row r="48">
@@ -1778,7 +1778,7 @@
         <v>1</v>
       </c>
       <c r="F48" t="n">
-        <v>0.9683012962341309</v>
+        <v>0.9755644798278809</v>
       </c>
     </row>
     <row r="49">
@@ -1806,7 +1806,7 @@
         <v>1</v>
       </c>
       <c r="F49" t="n">
-        <v>0.9930868744850159</v>
+        <v>0.9931508302688599</v>
       </c>
     </row>
     <row r="50">
@@ -1834,7 +1834,7 @@
         <v>1</v>
       </c>
       <c r="F50" t="n">
-        <v>0.961419939994812</v>
+        <v>0.9697245359420776</v>
       </c>
     </row>
     <row r="51">
@@ -1862,7 +1862,7 @@
         <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>0.9465126991271973</v>
+        <v>0.9572221040725708</v>
       </c>
     </row>
     <row r="52">
@@ -1890,7 +1890,7 @@
         <v>1</v>
       </c>
       <c r="F52" t="n">
-        <v>0.9899997115135193</v>
+        <v>0.9901753067970276</v>
       </c>
     </row>
     <row r="53">
@@ -1918,7 +1918,7 @@
         <v>1</v>
       </c>
       <c r="F53" t="n">
-        <v>0.961419939994812</v>
+        <v>0.9697245359420776</v>
       </c>
     </row>
     <row r="54">
@@ -1946,7 +1946,7 @@
         <v>0</v>
       </c>
       <c r="F54" t="n">
-        <v>0.9611994624137878</v>
+        <v>0.9695231318473816</v>
       </c>
     </row>
     <row r="55">
@@ -1974,7 +1974,7 @@
         <v>1</v>
       </c>
       <c r="F55" t="n">
-        <v>0.9916061162948608</v>
+        <v>0.9916859269142151</v>
       </c>
     </row>
     <row r="56">
@@ -2002,7 +2002,7 @@
         <v>1</v>
       </c>
       <c r="F56" t="n">
-        <v>0.9928051829338074</v>
+        <v>0.9928635954856873</v>
       </c>
     </row>
     <row r="57">
@@ -2030,7 +2030,7 @@
         <v>1</v>
       </c>
       <c r="F57" t="n">
-        <v>0.9930570125579834</v>
+        <v>0.9931139349937439</v>
       </c>
     </row>
     <row r="58">
@@ -2058,7 +2058,7 @@
         <v>1</v>
       </c>
       <c r="F58" t="n">
-        <v>0.9642336368560791</v>
+        <v>0.9685662388801575</v>
       </c>
     </row>
     <row r="59">
@@ -2086,7 +2086,7 @@
         <v>1</v>
       </c>
       <c r="F59" t="n">
-        <v>0.9930950999259949</v>
+        <v>0.9931837916374207</v>
       </c>
     </row>
     <row r="60">
@@ -2114,7 +2114,7 @@
         <v>1</v>
       </c>
       <c r="F60" t="n">
-        <v>0.9925329685211182</v>
+        <v>0.9926263689994812</v>
       </c>
     </row>
     <row r="61">
@@ -2142,7 +2142,7 @@
         <v>1</v>
       </c>
       <c r="F61" t="n">
-        <v>0.9926784038543701</v>
+        <v>0.9927504062652588</v>
       </c>
     </row>
     <row r="62">
@@ -2170,7 +2170,7 @@
         <v>1</v>
       </c>
       <c r="F62" t="n">
-        <v>0.9925278425216675</v>
+        <v>0.9925768971443176</v>
       </c>
     </row>
     <row r="63">
@@ -2198,7 +2198,7 @@
         <v>1</v>
       </c>
       <c r="F63" t="n">
-        <v>0.959704577922821</v>
+        <v>0.9646193981170654</v>
       </c>
     </row>
     <row r="64">
@@ -2226,7 +2226,7 @@
         <v>1</v>
       </c>
       <c r="F64" t="n">
-        <v>0.6526047587394714</v>
+        <v>0.6667877435684204</v>
       </c>
     </row>
     <row r="65">
@@ -2254,7 +2254,7 @@
         <v>1</v>
       </c>
       <c r="F65" t="n">
-        <v>0.9639434814453125</v>
+        <v>0.9685369729995728</v>
       </c>
     </row>
     <row r="66">
@@ -2282,7 +2282,7 @@
         <v>1</v>
       </c>
       <c r="F66" t="n">
-        <v>0.9639434814453125</v>
+        <v>0.9685369729995728</v>
       </c>
     </row>
     <row r="67">
@@ -2310,7 +2310,7 @@
         <v>1</v>
       </c>
       <c r="F67" t="n">
-        <v>0.9595982432365417</v>
+        <v>0.964400053024292</v>
       </c>
     </row>
     <row r="68">
@@ -2338,7 +2338,7 @@
         <v>1</v>
       </c>
       <c r="F68" t="n">
-        <v>0.9639434814453125</v>
+        <v>0.9685369729995728</v>
       </c>
     </row>
     <row r="69">
@@ -2366,7 +2366,7 @@
         <v>1</v>
       </c>
       <c r="F69" t="n">
-        <v>0.9505355954170227</v>
+        <v>0.9442524909973145</v>
       </c>
     </row>
     <row r="70">
@@ -2394,7 +2394,7 @@
         <v>1</v>
       </c>
       <c r="F70" t="n">
-        <v>0.991614818572998</v>
+        <v>0.9916873574256897</v>
       </c>
     </row>
     <row r="71">
@@ -2422,7 +2422,7 @@
         <v>0</v>
       </c>
       <c r="F71" t="n">
-        <v>0.9610488414764404</v>
+        <v>0.9655395746231079</v>
       </c>
     </row>
     <row r="72">
@@ -2450,7 +2450,7 @@
         <v>1</v>
       </c>
       <c r="F72" t="n">
-        <v>0.9881566166877747</v>
+        <v>0.9883644580841064</v>
       </c>
     </row>
     <row r="73">
@@ -2478,7 +2478,7 @@
         <v>1</v>
       </c>
       <c r="F73" t="n">
-        <v>0.9663239717483521</v>
+        <v>0.970529317855835</v>
       </c>
     </row>
     <row r="74">
@@ -2506,7 +2506,7 @@
         <v>1</v>
       </c>
       <c r="F74" t="n">
-        <v>0.9923404455184937</v>
+        <v>0.9924161434173584</v>
       </c>
     </row>
     <row r="75">
@@ -2534,7 +2534,7 @@
         <v>1</v>
       </c>
       <c r="F75" t="n">
-        <v>0.991050124168396</v>
+        <v>0.9911403059959412</v>
       </c>
     </row>
     <row r="76">
@@ -2562,7 +2562,7 @@
         <v>1</v>
       </c>
       <c r="F76" t="n">
-        <v>0.9663239717483521</v>
+        <v>0.970529317855835</v>
       </c>
     </row>
     <row r="77">
@@ -2590,7 +2590,7 @@
         <v>1</v>
       </c>
       <c r="F77" t="n">
-        <v>0.9900553226470947</v>
+        <v>0.9901695847511292</v>
       </c>
     </row>
     <row r="78">
@@ -2618,7 +2618,7 @@
         <v>1</v>
       </c>
       <c r="F78" t="n">
-        <v>0.9663239717483521</v>
+        <v>0.970529317855835</v>
       </c>
     </row>
     <row r="79">
@@ -2646,7 +2646,7 @@
         <v>1</v>
       </c>
       <c r="F79" t="n">
-        <v>0.992067813873291</v>
+        <v>0.9921352863311768</v>
       </c>
     </row>
     <row r="80">
@@ -2674,7 +2674,7 @@
         <v>1</v>
       </c>
       <c r="F80" t="n">
-        <v>0.9662925601005554</v>
+        <v>0.9705173969268799</v>
       </c>
     </row>
     <row r="81">
@@ -2702,7 +2702,7 @@
         <v>1</v>
       </c>
       <c r="F81" t="n">
-        <v>0.9901172518730164</v>
+        <v>0.990236222743988</v>
       </c>
     </row>
     <row r="82">
@@ -2730,7 +2730,7 @@
         <v>1</v>
       </c>
       <c r="F82" t="n">
-        <v>0.9662925601005554</v>
+        <v>0.9705173969268799</v>
       </c>
     </row>
     <row r="83">
@@ -2758,7 +2758,7 @@
         <v>1</v>
       </c>
       <c r="F83" t="n">
-        <v>0.9900745749473572</v>
+        <v>0.9901815056800842</v>
       </c>
     </row>
     <row r="84">
@@ -2786,7 +2786,7 @@
         <v>1</v>
       </c>
       <c r="F84" t="n">
-        <v>0.9900745749473572</v>
+        <v>0.9901815056800842</v>
       </c>
     </row>
     <row r="85">
@@ -2814,7 +2814,7 @@
         <v>1</v>
       </c>
       <c r="F85" t="n">
-        <v>0.9931648373603821</v>
+        <v>0.9932413101196289</v>
       </c>
     </row>
     <row r="86">
@@ -2842,7 +2842,7 @@
         <v>1</v>
       </c>
       <c r="F86" t="n">
-        <v>0.9676070213317871</v>
+        <v>0.9717167019844055</v>
       </c>
     </row>
     <row r="87">
@@ -2870,7 +2870,7 @@
         <v>1</v>
       </c>
       <c r="F87" t="n">
-        <v>0.991934061050415</v>
+        <v>0.9920401573181152</v>
       </c>
     </row>
     <row r="88">
@@ -2898,7 +2898,7 @@
         <v>1</v>
       </c>
       <c r="F88" t="n">
-        <v>0.9665279388427734</v>
+        <v>0.9707946181297302</v>
       </c>
     </row>
     <row r="89">
@@ -2926,7 +2926,7 @@
         <v>1</v>
       </c>
       <c r="F89" t="n">
-        <v>0.9900109171867371</v>
+        <v>0.9901551008224487</v>
       </c>
     </row>
     <row r="90">
@@ -2954,7 +2954,7 @@
         <v>1</v>
       </c>
       <c r="F90" t="n">
-        <v>0.9922671914100647</v>
+        <v>0.9923426508903503</v>
       </c>
     </row>
     <row r="91">
@@ -2982,7 +2982,7 @@
         <v>1</v>
       </c>
       <c r="F91" t="n">
-        <v>0.992258608341217</v>
+        <v>0.9923376441001892</v>
       </c>
     </row>
     <row r="92">
@@ -3010,7 +3010,7 @@
         <v>1</v>
       </c>
       <c r="F92" t="n">
-        <v>0.9922664761543274</v>
+        <v>0.9923409223556519</v>
       </c>
     </row>
     <row r="93">
@@ -3038,7 +3038,7 @@
         <v>1</v>
       </c>
       <c r="F93" t="n">
-        <v>0.9922519326210022</v>
+        <v>0.9923323392868042</v>
       </c>
     </row>
     <row r="94">
@@ -3066,7 +3066,7 @@
         <v>1</v>
       </c>
       <c r="F94" t="n">
-        <v>0.9922500848770142</v>
+        <v>0.9923291802406311</v>
       </c>
     </row>
     <row r="95">
@@ -3094,7 +3094,7 @@
         <v>1</v>
       </c>
       <c r="F95" t="n">
-        <v>0.9922508597373962</v>
+        <v>0.9923328161239624</v>
       </c>
     </row>
     <row r="96">
@@ -3122,7 +3122,7 @@
         <v>1</v>
       </c>
       <c r="F96" t="n">
-        <v>0.9930005073547363</v>
+        <v>0.9930576086044312</v>
       </c>
     </row>
     <row r="97">
@@ -3150,7 +3150,7 @@
         <v>1</v>
       </c>
       <c r="F97" t="n">
-        <v>0.811339259147644</v>
+        <v>0.6818398237228394</v>
       </c>
     </row>
     <row r="98">
@@ -3178,7 +3178,7 @@
         <v>1</v>
       </c>
       <c r="F98" t="n">
-        <v>0.9929794669151306</v>
+        <v>0.9930568933486938</v>
       </c>
     </row>
     <row r="99">
@@ -3206,7 +3206,7 @@
         <v>0</v>
       </c>
       <c r="F99" t="n">
-        <v>0.9426153302192688</v>
+        <v>0.945080578327179</v>
       </c>
     </row>
     <row r="100">
@@ -3234,7 +3234,7 @@
         <v>1</v>
       </c>
       <c r="F100" t="n">
-        <v>0.9916185736656189</v>
+        <v>0.9917145371437073</v>
       </c>
     </row>
     <row r="101">
@@ -3262,7 +3262,7 @@
         <v>1</v>
       </c>
       <c r="F101" t="n">
-        <v>0.9919419288635254</v>
+        <v>0.992023229598999</v>
       </c>
     </row>
     <row r="102">
@@ -3290,7 +3290,7 @@
         <v>1</v>
       </c>
       <c r="F102" t="n">
-        <v>0.8513273596763611</v>
+        <v>0.8145402669906616</v>
       </c>
     </row>
     <row r="103">
@@ -3318,7 +3318,7 @@
         <v>1</v>
       </c>
       <c r="F103" t="n">
-        <v>0.9667453765869141</v>
+        <v>0.9742709398269653</v>
       </c>
     </row>
     <row r="104">
@@ -3346,7 +3346,7 @@
         <v>1</v>
       </c>
       <c r="F104" t="n">
-        <v>0.9910600781440735</v>
+        <v>0.9911383986473083</v>
       </c>
     </row>
     <row r="105">
@@ -3374,7 +3374,7 @@
         <v>1</v>
       </c>
       <c r="F105" t="n">
-        <v>0.9507174491882324</v>
+        <v>0.9454655647277832</v>
       </c>
     </row>
     <row r="106">
@@ -3402,7 +3402,7 @@
         <v>1</v>
       </c>
       <c r="F106" t="n">
-        <v>0.9916326403617859</v>
+        <v>0.9916955828666687</v>
       </c>
     </row>
     <row r="107">
@@ -3430,7 +3430,7 @@
         <v>1</v>
       </c>
       <c r="F107" t="n">
-        <v>0.969506561756134</v>
+        <v>0.9766144156455994</v>
       </c>
     </row>
     <row r="108">
@@ -3458,7 +3458,7 @@
         <v>1</v>
       </c>
       <c r="F108" t="n">
-        <v>0.9420392513275146</v>
+        <v>0.919765293598175</v>
       </c>
     </row>
     <row r="109">
@@ -3486,7 +3486,7 @@
         <v>1</v>
       </c>
       <c r="F109" t="n">
-        <v>0.99208003282547</v>
+        <v>0.9921521544456482</v>
       </c>
     </row>
     <row r="110">
@@ -3514,7 +3514,7 @@
         <v>1</v>
       </c>
       <c r="F110" t="n">
-        <v>0.9900535345077515</v>
+        <v>0.9901875853538513</v>
       </c>
     </row>
     <row r="111">
@@ -3542,7 +3542,7 @@
         <v>1</v>
       </c>
       <c r="F111" t="n">
-        <v>0.9714592695236206</v>
+        <v>0.9781044125556946</v>
       </c>
     </row>
     <row r="112">
@@ -3570,7 +3570,7 @@
         <v>1</v>
       </c>
       <c r="F112" t="n">
-        <v>0.9683676958084106</v>
+        <v>0.9757585525512695</v>
       </c>
     </row>
     <row r="113">
@@ -3598,7 +3598,7 @@
         <v>1</v>
       </c>
       <c r="F113" t="n">
-        <v>0.9688736796379089</v>
+        <v>0.9727793335914612</v>
       </c>
     </row>
     <row r="114">
@@ -3626,7 +3626,7 @@
         <v>1</v>
       </c>
       <c r="F114" t="n">
-        <v>0.9925336837768555</v>
+        <v>0.9926103949546814</v>
       </c>
     </row>
     <row r="115">
@@ -3654,7 +3654,7 @@
         <v>1</v>
       </c>
       <c r="F115" t="n">
-        <v>0.9675046801567078</v>
+        <v>0.9714978337287903</v>
       </c>
     </row>
     <row r="116">
@@ -3682,7 +3682,7 @@
         <v>1</v>
       </c>
       <c r="F116" t="n">
-        <v>0.9898208379745483</v>
+        <v>0.9900355935096741</v>
       </c>
     </row>
     <row r="117">
@@ -3710,7 +3710,7 @@
         <v>1</v>
       </c>
       <c r="F117" t="n">
-        <v>0.9909555315971375</v>
+        <v>0.9910405278205872</v>
       </c>
     </row>
     <row r="118">
@@ -3738,7 +3738,7 @@
         <v>1</v>
       </c>
       <c r="F118" t="n">
-        <v>0.8230662941932678</v>
+        <v>0.7899017333984375</v>
       </c>
     </row>
     <row r="119">
@@ -3766,7 +3766,7 @@
         <v>0</v>
       </c>
       <c r="F119" t="n">
-        <v>0.8916419148445129</v>
+        <v>0.9086796641349792</v>
       </c>
     </row>
     <row r="120">
@@ -3794,7 +3794,7 @@
         <v>1</v>
       </c>
       <c r="F120" t="n">
-        <v>0.9900535345077515</v>
+        <v>0.9901875853538513</v>
       </c>
     </row>
     <row r="121">
@@ -3822,7 +3822,7 @@
         <v>1</v>
       </c>
       <c r="F121" t="n">
-        <v>0.9508660435676575</v>
+        <v>0.9442043304443359</v>
       </c>
     </row>
     <row r="122">
@@ -3850,7 +3850,7 @@
         <v>1</v>
       </c>
       <c r="F122" t="n">
-        <v>0.992980420589447</v>
+        <v>0.9930418729782104</v>
       </c>
     </row>
     <row r="123">
@@ -3878,7 +3878,7 @@
         <v>1</v>
       </c>
       <c r="F123" t="n">
-        <v>0.9508660435676575</v>
+        <v>0.9442043304443359</v>
       </c>
     </row>
     <row r="124">
@@ -3906,7 +3906,7 @@
         <v>1</v>
       </c>
       <c r="F124" t="n">
-        <v>0.992980420589447</v>
+        <v>0.9930418729782104</v>
       </c>
     </row>
     <row r="125">
@@ -3934,7 +3934,7 @@
         <v>1</v>
       </c>
       <c r="F125" t="n">
-        <v>0.9508660435676575</v>
+        <v>0.9442043304443359</v>
       </c>
     </row>
     <row r="126">
@@ -3962,7 +3962,7 @@
         <v>1</v>
       </c>
       <c r="F126" t="n">
-        <v>0.9929627776145935</v>
+        <v>0.9930155277252197</v>
       </c>
     </row>
     <row r="127">
@@ -3990,7 +3990,7 @@
         <v>0</v>
       </c>
       <c r="F127" t="n">
-        <v>0.7814671397209167</v>
+        <v>0.7509148716926575</v>
       </c>
     </row>
     <row r="128">
@@ -4018,7 +4018,7 @@
         <v>1</v>
       </c>
       <c r="F128" t="n">
-        <v>0.9900535345077515</v>
+        <v>0.9901875853538513</v>
       </c>
     </row>
     <row r="129">
@@ -4046,7 +4046,7 @@
         <v>1</v>
       </c>
       <c r="F129" t="n">
-        <v>0.9885894060134888</v>
+        <v>0.9888930916786194</v>
       </c>
     </row>
     <row r="130">
@@ -4074,7 +4074,7 @@
         <v>0</v>
       </c>
       <c r="F130" t="n">
-        <v>0.7566537261009216</v>
+        <v>0.6907042860984802</v>
       </c>
     </row>
     <row r="131">
@@ -4102,7 +4102,7 @@
         <v>1</v>
       </c>
       <c r="F131" t="n">
-        <v>0.9910629987716675</v>
+        <v>0.9911575317382812</v>
       </c>
     </row>
     <row r="132">
@@ -4130,7 +4130,7 @@
         <v>1</v>
       </c>
       <c r="F132" t="n">
-        <v>0.4880706667900085</v>
+        <v>0.396036684513092</v>
       </c>
     </row>
     <row r="133">
@@ -4158,7 +4158,7 @@
         <v>1</v>
       </c>
       <c r="F133" t="n">
-        <v>0.9909647703170776</v>
+        <v>0.9910869002342224</v>
       </c>
     </row>
     <row r="134">
@@ -4186,7 +4186,7 @@
         <v>0</v>
       </c>
       <c r="F134" t="n">
-        <v>0.9923620223999023</v>
+        <v>0.992420494556427</v>
       </c>
     </row>
     <row r="135">
@@ -4214,7 +4214,7 @@
         <v>1</v>
       </c>
       <c r="F135" t="n">
-        <v>0.9916903972625732</v>
+        <v>0.9917489290237427</v>
       </c>
     </row>
     <row r="136">
@@ -4242,7 +4242,7 @@
         <v>1</v>
       </c>
       <c r="F136" t="n">
-        <v>0.9881582856178284</v>
+        <v>0.9885703921318054</v>
       </c>
     </row>
     <row r="137">
@@ -4270,7 +4270,7 @@
         <v>1</v>
       </c>
       <c r="F137" t="n">
-        <v>0.9910854697227478</v>
+        <v>0.9911925196647644</v>
       </c>
     </row>
     <row r="138">
@@ -4298,7 +4298,7 @@
         <v>1</v>
       </c>
       <c r="F138" t="n">
-        <v>0.9910107851028442</v>
+        <v>0.9911296367645264</v>
       </c>
     </row>
     <row r="139">
@@ -4326,7 +4326,7 @@
         <v>1</v>
       </c>
       <c r="F139" t="n">
-        <v>0.991089940071106</v>
+        <v>0.9911971092224121</v>
       </c>
     </row>
     <row r="140">
@@ -4354,7 +4354,7 @@
         <v>1</v>
       </c>
       <c r="F140" t="n">
-        <v>0.9901718497276306</v>
+        <v>0.9902978539466858</v>
       </c>
     </row>
     <row r="141">
@@ -4382,7 +4382,7 @@
         <v>1</v>
       </c>
       <c r="F141" t="n">
-        <v>0.9921858310699463</v>
+        <v>0.992442786693573</v>
       </c>
     </row>
     <row r="142">
@@ -4410,7 +4410,7 @@
         <v>1</v>
       </c>
       <c r="F142" t="n">
-        <v>0.9900535345077515</v>
+        <v>0.9901875853538513</v>
       </c>
     </row>
     <row r="143">
@@ -4438,7 +4438,7 @@
         <v>1</v>
       </c>
       <c r="F143" t="n">
-        <v>0.9635873436927795</v>
+        <v>0.9680639505386353</v>
       </c>
     </row>
     <row r="144">
@@ -4466,7 +4466,7 @@
         <v>1</v>
       </c>
       <c r="F144" t="n">
-        <v>0.9924861192703247</v>
+        <v>0.9925591945648193</v>
       </c>
     </row>
     <row r="145">
@@ -4494,7 +4494,7 @@
         <v>1</v>
       </c>
       <c r="F145" t="n">
-        <v>0.9635873436927795</v>
+        <v>0.9680639505386353</v>
       </c>
     </row>
     <row r="146">
@@ -4522,7 +4522,7 @@
         <v>1</v>
       </c>
       <c r="F146" t="n">
-        <v>0.9900161623954773</v>
+        <v>0.9901522994041443</v>
       </c>
     </row>
     <row r="147">
@@ -4550,7 +4550,7 @@
         <v>1</v>
       </c>
       <c r="F147" t="n">
-        <v>0.9505355954170227</v>
+        <v>0.9442524909973145</v>
       </c>
     </row>
     <row r="148">
@@ -4578,7 +4578,7 @@
         <v>1</v>
       </c>
       <c r="F148" t="n">
-        <v>0.991986870765686</v>
+        <v>0.9920530319213867</v>
       </c>
     </row>
     <row r="149">
@@ -4606,7 +4606,7 @@
         <v>1</v>
       </c>
       <c r="F149" t="n">
-        <v>0.964659571647644</v>
+        <v>0.969074547290802</v>
       </c>
     </row>
     <row r="150">
@@ -4634,7 +4634,7 @@
         <v>1</v>
       </c>
       <c r="F150" t="n">
-        <v>0.8805937170982361</v>
+        <v>0.8615320324897766</v>
       </c>
     </row>
     <row r="151">
@@ -4662,7 +4662,7 @@
         <v>1</v>
       </c>
       <c r="F151" t="n">
-        <v>0.9900535345077515</v>
+        <v>0.9901875853538513</v>
       </c>
     </row>
     <row r="152">
@@ -4690,7 +4690,7 @@
         <v>1</v>
       </c>
       <c r="F152" t="n">
-        <v>0.7822718620300293</v>
+        <v>0.7764051556587219</v>
       </c>
     </row>
     <row r="153">
@@ -4718,7 +4718,7 @@
         <v>1</v>
       </c>
       <c r="F153" t="n">
-        <v>0.9928489923477173</v>
+        <v>0.9929078817367554</v>
       </c>
     </row>
     <row r="154">
@@ -4746,7 +4746,7 @@
         <v>1</v>
       </c>
       <c r="F154" t="n">
-        <v>0.941520094871521</v>
+        <v>0.9189469218254089</v>
       </c>
     </row>
     <row r="155">
@@ -4774,7 +4774,7 @@
         <v>1</v>
       </c>
       <c r="F155" t="n">
-        <v>0.9923405647277832</v>
+        <v>0.9924128651618958</v>
       </c>
     </row>
     <row r="156">
@@ -4802,7 +4802,7 @@
         <v>1</v>
       </c>
       <c r="F156" t="n">
-        <v>0.9416447281837463</v>
+        <v>0.9190235733985901</v>
       </c>
     </row>
     <row r="157">
@@ -4830,7 +4830,7 @@
         <v>1</v>
       </c>
       <c r="F157" t="n">
-        <v>0.9925203323364258</v>
+        <v>0.9925946593284607</v>
       </c>
     </row>
     <row r="158">
@@ -4858,7 +4858,7 @@
         <v>1</v>
       </c>
       <c r="F158" t="n">
-        <v>0.9418360590934753</v>
+        <v>0.9192238450050354</v>
       </c>
     </row>
     <row r="159">
@@ -4886,7 +4886,7 @@
         <v>1</v>
       </c>
       <c r="F159" t="n">
-        <v>0.9926048517227173</v>
+        <v>0.9926825165748596</v>
       </c>
     </row>
     <row r="160">
@@ -4914,7 +4914,7 @@
         <v>1</v>
       </c>
       <c r="F160" t="n">
-        <v>0.95792555809021</v>
+        <v>0.9608413577079773</v>
       </c>
     </row>
     <row r="161">
@@ -4942,7 +4942,7 @@
         <v>1</v>
       </c>
       <c r="F161" t="n">
-        <v>0.9919701218605042</v>
+        <v>0.9920490384101868</v>
       </c>
     </row>
     <row r="162">
@@ -4970,7 +4970,7 @@
         <v>0</v>
       </c>
       <c r="F162" t="n">
-        <v>0.9916937947273254</v>
+        <v>0.9916979074478149</v>
       </c>
     </row>
     <row r="163">
@@ -4998,7 +4998,7 @@
         <v>1</v>
       </c>
       <c r="F163" t="n">
-        <v>0.991068959236145</v>
+        <v>0.9911961555480957</v>
       </c>
     </row>
     <row r="164">
@@ -5026,7 +5026,7 @@
         <v>1</v>
       </c>
       <c r="F164" t="n">
-        <v>0.9634148478507996</v>
+        <v>0.9675512909889221</v>
       </c>
     </row>
     <row r="165">
@@ -5054,7 +5054,7 @@
         <v>1</v>
       </c>
       <c r="F165" t="n">
-        <v>0.9929593801498413</v>
+        <v>0.9930181503295898</v>
       </c>
     </row>
     <row r="166">
@@ -5082,7 +5082,7 @@
         <v>0</v>
       </c>
       <c r="F166" t="n">
-        <v>0.9553748965263367</v>
+        <v>0.9585237503051758</v>
       </c>
     </row>
     <row r="167">
@@ -5110,7 +5110,7 @@
         <v>1</v>
       </c>
       <c r="F167" t="n">
-        <v>0.965330958366394</v>
+        <v>0.9731586575508118</v>
       </c>
     </row>
     <row r="168">
@@ -5138,7 +5138,7 @@
         <v>0</v>
       </c>
       <c r="F168" t="n">
-        <v>0.9687711596488953</v>
+        <v>0.9726055264472961</v>
       </c>
     </row>
     <row r="169">
@@ -5166,7 +5166,7 @@
         <v>1</v>
       </c>
       <c r="F169" t="n">
-        <v>0.9900535345077515</v>
+        <v>0.9901875853538513</v>
       </c>
     </row>
     <row r="170">
@@ -5194,7 +5194,7 @@
         <v>1</v>
       </c>
       <c r="F170" t="n">
-        <v>0.965330958366394</v>
+        <v>0.9731586575508118</v>
       </c>
     </row>
     <row r="171">
@@ -5222,7 +5222,7 @@
         <v>0</v>
       </c>
       <c r="F171" t="n">
-        <v>0.9672278761863708</v>
+        <v>0.971095085144043</v>
       </c>
     </row>
     <row r="172">
@@ -5250,7 +5250,7 @@
         <v>1</v>
       </c>
       <c r="F172" t="n">
-        <v>0.9900535345077515</v>
+        <v>0.9901875853538513</v>
       </c>
     </row>
     <row r="173">
@@ -5278,7 +5278,7 @@
         <v>1</v>
       </c>
       <c r="F173" t="n">
-        <v>0.9910570383071899</v>
+        <v>0.9911535382270813</v>
       </c>
     </row>
     <row r="174">
@@ -5306,7 +5306,7 @@
         <v>1</v>
       </c>
       <c r="F174" t="n">
-        <v>0.9910661578178406</v>
+        <v>0.9911729693412781</v>
       </c>
     </row>
     <row r="175">
@@ -5334,7 +5334,7 @@
         <v>1</v>
       </c>
       <c r="F175" t="n">
-        <v>0.9910570383071899</v>
+        <v>0.9911535382270813</v>
       </c>
     </row>
     <row r="176">
@@ -5362,7 +5362,7 @@
         <v>1</v>
       </c>
       <c r="F176" t="n">
-        <v>0.9910570383071899</v>
+        <v>0.9911535382270813</v>
       </c>
     </row>
     <row r="177">
@@ -5390,7 +5390,7 @@
         <v>1</v>
       </c>
       <c r="F177" t="n">
-        <v>0.9910661578178406</v>
+        <v>0.9911729693412781</v>
       </c>
     </row>
     <row r="178">
@@ -5418,7 +5418,7 @@
         <v>1</v>
       </c>
       <c r="F178" t="n">
-        <v>0.992031455039978</v>
+        <v>0.9921046495437622</v>
       </c>
     </row>
     <row r="179">
@@ -5446,7 +5446,7 @@
         <v>1</v>
       </c>
       <c r="F179" t="n">
-        <v>0.9883009791374207</v>
+        <v>0.9884917736053467</v>
       </c>
     </row>
     <row r="180">
@@ -5474,7 +5474,7 @@
         <v>1</v>
       </c>
       <c r="F180" t="n">
-        <v>0.9910333752632141</v>
+        <v>0.9911422729492188</v>
       </c>
     </row>
     <row r="181">
@@ -5502,7 +5502,7 @@
         <v>1</v>
       </c>
       <c r="F181" t="n">
-        <v>0.9921168684959412</v>
+        <v>0.9921745657920837</v>
       </c>
     </row>
     <row r="182">
@@ -5530,7 +5530,7 @@
         <v>1</v>
       </c>
       <c r="F182" t="n">
-        <v>0.9916000366210938</v>
+        <v>0.9916833639144897</v>
       </c>
     </row>
     <row r="183">
@@ -5558,7 +5558,7 @@
         <v>1</v>
       </c>
       <c r="F183" t="n">
-        <v>0.9525659084320068</v>
+        <v>0.9467311501502991</v>
       </c>
     </row>
     <row r="184">
@@ -5586,7 +5586,7 @@
         <v>1</v>
       </c>
       <c r="F184" t="n">
-        <v>0.9925798773765564</v>
+        <v>0.9926209449768066</v>
       </c>
     </row>
     <row r="185">
@@ -5614,7 +5614,7 @@
         <v>1</v>
       </c>
       <c r="F185" t="n">
-        <v>0.9925549626350403</v>
+        <v>0.9926177859306335</v>
       </c>
     </row>
     <row r="186">
@@ -5642,7 +5642,7 @@
         <v>1</v>
       </c>
       <c r="F186" t="n">
-        <v>0.9926445484161377</v>
+        <v>0.9927151799201965</v>
       </c>
     </row>
     <row r="187">
@@ -5670,7 +5670,7 @@
         <v>1</v>
       </c>
       <c r="F187" t="n">
-        <v>0.992634117603302</v>
+        <v>0.9926993250846863</v>
       </c>
     </row>
     <row r="188">
@@ -5698,7 +5698,7 @@
         <v>1</v>
       </c>
       <c r="F188" t="n">
-        <v>0.9920017719268799</v>
+        <v>0.9920769929885864</v>
       </c>
     </row>
     <row r="189">
@@ -5726,7 +5726,7 @@
         <v>1</v>
       </c>
       <c r="F189" t="n">
-        <v>0.9922028779983521</v>
+        <v>0.9922707080841064</v>
       </c>
     </row>
     <row r="190">
@@ -5754,7 +5754,7 @@
         <v>1</v>
       </c>
       <c r="F190" t="n">
-        <v>0.9921935796737671</v>
+        <v>0.9922673106193542</v>
       </c>
     </row>
     <row r="191">
@@ -5782,7 +5782,7 @@
         <v>1</v>
       </c>
       <c r="F191" t="n">
-        <v>0.7861914038658142</v>
+        <v>0.6715330481529236</v>
       </c>
     </row>
     <row r="192">
@@ -5810,7 +5810,7 @@
         <v>1</v>
       </c>
       <c r="F192" t="n">
-        <v>0.9916879534721375</v>
+        <v>0.9917612075805664</v>
       </c>
     </row>
     <row r="193">
@@ -5838,7 +5838,7 @@
         <v>1</v>
       </c>
       <c r="F193" t="n">
-        <v>0.9911189675331116</v>
+        <v>0.9912039041519165</v>
       </c>
     </row>
     <row r="194">
@@ -5866,7 +5866,7 @@
         <v>1</v>
       </c>
       <c r="F194" t="n">
-        <v>0.9464101791381836</v>
+        <v>0.9403685927391052</v>
       </c>
     </row>
     <row r="195">
@@ -5894,7 +5894,7 @@
         <v>1</v>
       </c>
       <c r="F195" t="n">
-        <v>0.9717474579811096</v>
+        <v>0.9787002205848694</v>
       </c>
     </row>
     <row r="196">
@@ -5922,7 +5922,7 @@
         <v>1</v>
       </c>
       <c r="F196" t="n">
-        <v>0.9925969839096069</v>
+        <v>0.9926518797874451</v>
       </c>
     </row>
     <row r="197">
@@ -5950,7 +5950,7 @@
         <v>1</v>
       </c>
       <c r="F197" t="n">
-        <v>0.9926734566688538</v>
+        <v>0.9927371144294739</v>
       </c>
     </row>
     <row r="198">
@@ -5978,7 +5978,7 @@
         <v>1</v>
       </c>
       <c r="F198" t="n">
-        <v>0.9927985668182373</v>
+        <v>0.9928520321846008</v>
       </c>
     </row>
     <row r="199">
@@ -6006,7 +6006,7 @@
         <v>1</v>
       </c>
       <c r="F199" t="n">
-        <v>0.9919747710227966</v>
+        <v>0.9920370578765869</v>
       </c>
     </row>
     <row r="200">
@@ -6034,7 +6034,7 @@
         <v>0</v>
       </c>
       <c r="F200" t="n">
-        <v>0.89615797996521</v>
+        <v>0.9076738953590393</v>
       </c>
     </row>
     <row r="201">
@@ -6062,7 +6062,7 @@
         <v>1</v>
       </c>
       <c r="F201" t="n">
-        <v>0.9919706583023071</v>
+        <v>0.9920430779457092</v>
       </c>
     </row>
     <row r="202">
@@ -6090,7 +6090,7 @@
         <v>1</v>
       </c>
       <c r="F202" t="n">
-        <v>0.9921370148658752</v>
+        <v>0.9921777844429016</v>
       </c>
     </row>
     <row r="203">
@@ -6118,7 +6118,7 @@
         <v>1</v>
       </c>
       <c r="F203" t="n">
-        <v>0.9910889863967896</v>
+        <v>0.9911950826644897</v>
       </c>
     </row>
     <row r="204">
@@ -6146,7 +6146,7 @@
         <v>1</v>
       </c>
       <c r="F204" t="n">
-        <v>0.9656707644462585</v>
+        <v>0.9733466506004333</v>
       </c>
     </row>
     <row r="205">
@@ -6174,7 +6174,7 @@
         <v>1</v>
       </c>
       <c r="F205" t="n">
-        <v>0.9928690791130066</v>
+        <v>0.9929448962211609</v>
       </c>
     </row>
     <row r="206">
@@ -6202,7 +6202,7 @@
         <v>1</v>
       </c>
       <c r="F206" t="n">
-        <v>0.9909909963607788</v>
+        <v>0.9910957813262939</v>
       </c>
     </row>
     <row r="207">
@@ -6230,7 +6230,7 @@
         <v>1</v>
       </c>
       <c r="F207" t="n">
-        <v>0.8130666017532349</v>
+        <v>0.6837595701217651</v>
       </c>
     </row>
     <row r="208">
@@ -6258,7 +6258,7 @@
         <v>1</v>
       </c>
       <c r="F208" t="n">
-        <v>0.9882116913795471</v>
+        <v>0.9884346723556519</v>
       </c>
     </row>
     <row r="209">
@@ -6286,7 +6286,7 @@
         <v>1</v>
       </c>
       <c r="F209" t="n">
-        <v>0.7358524799346924</v>
+        <v>0.63709557056427</v>
       </c>
     </row>
     <row r="210">
@@ -6314,7 +6314,7 @@
         <v>1</v>
       </c>
       <c r="F210" t="n">
-        <v>0.9909994006156921</v>
+        <v>0.9911221265792847</v>
       </c>
     </row>
   </sheetData>

</xml_diff>